<commit_message>
Removed non-start year prices for plants subject to endogenous learning
</commit_message>
<xml_diff>
--- a/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
+++ b/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EvelineDB\Dropbox\Projeto EPS-WRI\elec_Eveline\Apil 2020\variables corrected\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\elec\CCaMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3FB43E-90AA-4F49-A5BF-F301A2277284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12578" tabRatio="653"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -24,7 +23,7 @@
   <externalReferences>
     <externalReference r:id="rId8"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -408,13 +407,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -623,7 +622,7 @@
       <name val="AdvOT596495f2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -663,6 +662,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,28 +840,28 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -953,10 +958,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -974,7 +979,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -992,10 +997,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1003,10 +1008,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1014,10 +1019,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1025,10 +1030,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1036,10 +1041,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1047,10 +1052,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1058,15 +1063,15 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1092,7 +1097,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1100,7 +1105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1125,7 +1130,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1149,6 +1154,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1157,234 +1163,234 @@
     </xf>
   </cellXfs>
   <cellStyles count="228">
-    <cellStyle name="20% - Accent1 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent1 2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2" xfId="151" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2" xfId="173" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2 2" xfId="217" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 3" xfId="195" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - Accent1 2 2 3" xfId="162" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - Accent1 2 2 3 2" xfId="206" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - Accent1 2 2 4" xfId="184" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent2 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2" xfId="152" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2" xfId="174" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2 2" xfId="218" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 3" xfId="196" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="20% - Accent2 2 2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="20% - Accent2 2 2 3 2" xfId="207" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="20% - Accent2 2 2 4" xfId="185" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="20% - Accent3 2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="20% - Accent3 2 2 2" xfId="153" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="20% - Accent3 2 2 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="20% - Accent3 2 2 2 2 2" xfId="219" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="20% - Accent3 2 2 2 3" xfId="197" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="20% - Accent3 2 2 3" xfId="164" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="20% - Accent3 2 2 3 2" xfId="208" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="20% - Accent3 2 2 4" xfId="186" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="20% - Accent4 2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="20% - Accent4 2 2 2" xfId="154" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="20% - Accent4 2 2 2 2" xfId="176" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="20% - Accent4 2 2 2 2 2" xfId="220" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="20% - Accent4 2 2 2 3" xfId="198" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="20% - Accent4 2 2 3" xfId="165" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="20% - Accent4 2 2 3 2" xfId="209" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="20% - Accent4 2 2 4" xfId="187" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Calculated" xfId="24" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Comma 10" xfId="25" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Comma 10 2" xfId="155" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Comma 10 2 2" xfId="177" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Comma 10 2 2 2" xfId="221" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Comma 10 2 3" xfId="199" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Comma 10 3" xfId="166" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Comma 10 3 2" xfId="210" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Comma 10 4" xfId="188" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Comma 11" xfId="26" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Comma 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Comma 2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Comma 2 2 2" xfId="156" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Comma 2 2 2 2" xfId="178" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Comma 2 2 2 2 2" xfId="222" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Comma 2 2 2 3" xfId="200" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Comma 2 2 3" xfId="167" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Comma 2 2 3 2" xfId="211" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Comma 2 2 4" xfId="189" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Comma 3" xfId="29" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Comma 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Comma 3 2 2" xfId="157" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Comma 3 2 2 2" xfId="179" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Comma 3 2 2 2 2" xfId="223" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Comma 3 2 2 3" xfId="201" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Comma 3 2 3" xfId="168" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Comma 3 2 3 2" xfId="212" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Comma 3 2 4" xfId="190" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Comma 4" xfId="31" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Comma 5" xfId="32" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Comma 6" xfId="33" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Comma 7" xfId="34" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Comma 8" xfId="35" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Comma 9" xfId="36" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Currency 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Currency 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Currency 4" xfId="39" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Currency 5" xfId="40" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Currency 6" xfId="41" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Currency 7" xfId="42" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Currency 8" xfId="43" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Currency 8 2" xfId="158" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Currency 8 2 2" xfId="180" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Currency 8 2 2 2" xfId="224" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Currency 8 2 3" xfId="202" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Currency 8 3" xfId="169" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Currency 8 3 2" xfId="213" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Currency 8 4" xfId="191" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Footnotes: all except top row" xfId="9" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Header: bottom row" xfId="2" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Header: top rows" xfId="10" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Heading" xfId="44" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Heading 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Heading2" xfId="46" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Hiperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 10" xfId="47" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Hyperlink 10 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Hyperlink 10 3" xfId="49" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Hyperlink 11" xfId="50" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Hyperlink 11 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Hyperlink 11 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Hyperlink 12" xfId="53" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Hyperlink 12 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Hyperlink 12 3" xfId="55" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Hyperlink 13" xfId="56" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Hyperlink 13 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Hyperlink 13 3" xfId="58" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Hyperlink 14" xfId="59" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Hyperlink 14 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Hyperlink 14 3" xfId="61" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Hyperlink 15" xfId="62" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Hyperlink 15 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Hyperlink 15 3" xfId="64" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Hyperlink 16" xfId="65" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Hyperlink 16 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Hyperlink 16 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Hyperlink 17" xfId="68" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Hyperlink 17 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Hyperlink 17 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Hyperlink 18" xfId="71" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Hyperlink 18 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Hyperlink 18 3" xfId="73" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Hyperlink 19" xfId="74" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Hyperlink 19 2" xfId="75" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Hyperlink 19 3" xfId="76" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Hyperlink 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Hyperlink 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Hyperlink 2 4" xfId="77" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Hyperlink 20" xfId="80" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Hyperlink 20 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Hyperlink 20 3" xfId="82" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Hyperlink 21" xfId="83" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Hyperlink 21 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Hyperlink 21 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Hyperlink 22" xfId="86" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Hyperlink 22 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Hyperlink 22 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Hyperlink 23" xfId="89" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Hyperlink 23 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Hyperlink 23 3" xfId="91" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Hyperlink 24" xfId="92" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Hyperlink 25" xfId="93" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Hyperlink 26" xfId="94" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Hyperlink 27" xfId="95" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Hyperlink 28" xfId="96" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Hyperlink 29" xfId="97" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Hyperlink 3 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Hyperlink 3 3" xfId="100" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Hyperlink 30" xfId="101" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Hyperlink 31" xfId="102" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Hyperlink 32" xfId="103" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Hyperlink 33" xfId="104" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Hyperlink 33 2" xfId="105" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Hyperlink 33 3" xfId="106" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Hyperlink 34" xfId="107" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Hyperlink 34 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Hyperlink 34 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Hyperlink 34 4" xfId="110" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Hyperlink 34 5" xfId="111" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="Hyperlink 4" xfId="112" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Hyperlink 4 2" xfId="113" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Hyperlink 4 3" xfId="114" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="Hyperlink 5" xfId="115" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="Hyperlink 5 2" xfId="116" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="Hyperlink 5 3" xfId="117" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="Hyperlink 6" xfId="118" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="Hyperlink 6 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="Hyperlink 6 3" xfId="120" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="Hyperlink 7" xfId="121" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="Hyperlink 7 2" xfId="122" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="Hyperlink 7 3" xfId="123" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="Hyperlink 8" xfId="124" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="Hyperlink 8 2" xfId="125" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="Hyperlink 8 3" xfId="126" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="Hyperlink 9" xfId="127" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="Hyperlink 9 2" xfId="128" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="Hyperlink 9 3" xfId="129" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="Input 2" xfId="130" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="Linked" xfId="131" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="16"/>
+    <cellStyle name="20% - Accent1 2 2" xfId="17"/>
+    <cellStyle name="20% - Accent1 2 2 2" xfId="151"/>
+    <cellStyle name="20% - Accent1 2 2 2 2" xfId="173"/>
+    <cellStyle name="20% - Accent1 2 2 2 2 2" xfId="217"/>
+    <cellStyle name="20% - Accent1 2 2 2 3" xfId="195"/>
+    <cellStyle name="20% - Accent1 2 2 3" xfId="162"/>
+    <cellStyle name="20% - Accent1 2 2 3 2" xfId="206"/>
+    <cellStyle name="20% - Accent1 2 2 4" xfId="184"/>
+    <cellStyle name="20% - Accent2 2" xfId="18"/>
+    <cellStyle name="20% - Accent2 2 2" xfId="19"/>
+    <cellStyle name="20% - Accent2 2 2 2" xfId="152"/>
+    <cellStyle name="20% - Accent2 2 2 2 2" xfId="174"/>
+    <cellStyle name="20% - Accent2 2 2 2 2 2" xfId="218"/>
+    <cellStyle name="20% - Accent2 2 2 2 3" xfId="196"/>
+    <cellStyle name="20% - Accent2 2 2 3" xfId="163"/>
+    <cellStyle name="20% - Accent2 2 2 3 2" xfId="207"/>
+    <cellStyle name="20% - Accent2 2 2 4" xfId="185"/>
+    <cellStyle name="20% - Accent3 2" xfId="20"/>
+    <cellStyle name="20% - Accent3 2 2" xfId="21"/>
+    <cellStyle name="20% - Accent3 2 2 2" xfId="153"/>
+    <cellStyle name="20% - Accent3 2 2 2 2" xfId="175"/>
+    <cellStyle name="20% - Accent3 2 2 2 2 2" xfId="219"/>
+    <cellStyle name="20% - Accent3 2 2 2 3" xfId="197"/>
+    <cellStyle name="20% - Accent3 2 2 3" xfId="164"/>
+    <cellStyle name="20% - Accent3 2 2 3 2" xfId="208"/>
+    <cellStyle name="20% - Accent3 2 2 4" xfId="186"/>
+    <cellStyle name="20% - Accent4 2" xfId="22"/>
+    <cellStyle name="20% - Accent4 2 2" xfId="23"/>
+    <cellStyle name="20% - Accent4 2 2 2" xfId="154"/>
+    <cellStyle name="20% - Accent4 2 2 2 2" xfId="176"/>
+    <cellStyle name="20% - Accent4 2 2 2 2 2" xfId="220"/>
+    <cellStyle name="20% - Accent4 2 2 2 3" xfId="198"/>
+    <cellStyle name="20% - Accent4 2 2 3" xfId="165"/>
+    <cellStyle name="20% - Accent4 2 2 3 2" xfId="209"/>
+    <cellStyle name="20% - Accent4 2 2 4" xfId="187"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Calculated" xfId="24"/>
+    <cellStyle name="Comma 10" xfId="25"/>
+    <cellStyle name="Comma 10 2" xfId="155"/>
+    <cellStyle name="Comma 10 2 2" xfId="177"/>
+    <cellStyle name="Comma 10 2 2 2" xfId="221"/>
+    <cellStyle name="Comma 10 2 3" xfId="199"/>
+    <cellStyle name="Comma 10 3" xfId="166"/>
+    <cellStyle name="Comma 10 3 2" xfId="210"/>
+    <cellStyle name="Comma 10 4" xfId="188"/>
+    <cellStyle name="Comma 11" xfId="26"/>
+    <cellStyle name="Comma 2" xfId="27"/>
+    <cellStyle name="Comma 2 2" xfId="28"/>
+    <cellStyle name="Comma 2 2 2" xfId="156"/>
+    <cellStyle name="Comma 2 2 2 2" xfId="178"/>
+    <cellStyle name="Comma 2 2 2 2 2" xfId="222"/>
+    <cellStyle name="Comma 2 2 2 3" xfId="200"/>
+    <cellStyle name="Comma 2 2 3" xfId="167"/>
+    <cellStyle name="Comma 2 2 3 2" xfId="211"/>
+    <cellStyle name="Comma 2 2 4" xfId="189"/>
+    <cellStyle name="Comma 3" xfId="29"/>
+    <cellStyle name="Comma 3 2" xfId="30"/>
+    <cellStyle name="Comma 3 2 2" xfId="157"/>
+    <cellStyle name="Comma 3 2 2 2" xfId="179"/>
+    <cellStyle name="Comma 3 2 2 2 2" xfId="223"/>
+    <cellStyle name="Comma 3 2 2 3" xfId="201"/>
+    <cellStyle name="Comma 3 2 3" xfId="168"/>
+    <cellStyle name="Comma 3 2 3 2" xfId="212"/>
+    <cellStyle name="Comma 3 2 4" xfId="190"/>
+    <cellStyle name="Comma 4" xfId="31"/>
+    <cellStyle name="Comma 5" xfId="32"/>
+    <cellStyle name="Comma 6" xfId="33"/>
+    <cellStyle name="Comma 7" xfId="34"/>
+    <cellStyle name="Comma 8" xfId="35"/>
+    <cellStyle name="Comma 9" xfId="36"/>
+    <cellStyle name="Currency 2" xfId="37"/>
+    <cellStyle name="Currency 3" xfId="38"/>
+    <cellStyle name="Currency 4" xfId="39"/>
+    <cellStyle name="Currency 5" xfId="40"/>
+    <cellStyle name="Currency 6" xfId="41"/>
+    <cellStyle name="Currency 7" xfId="42"/>
+    <cellStyle name="Currency 8" xfId="43"/>
+    <cellStyle name="Currency 8 2" xfId="158"/>
+    <cellStyle name="Currency 8 2 2" xfId="180"/>
+    <cellStyle name="Currency 8 2 2 2" xfId="224"/>
+    <cellStyle name="Currency 8 2 3" xfId="202"/>
+    <cellStyle name="Currency 8 3" xfId="169"/>
+    <cellStyle name="Currency 8 3 2" xfId="213"/>
+    <cellStyle name="Currency 8 4" xfId="191"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Footnotes: all except top row" xfId="9"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="2"/>
+    <cellStyle name="Header: top rows" xfId="10"/>
+    <cellStyle name="Heading" xfId="44"/>
+    <cellStyle name="Heading 2 2" xfId="45"/>
+    <cellStyle name="Heading2" xfId="46"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
+    <cellStyle name="Hyperlink 10" xfId="47"/>
+    <cellStyle name="Hyperlink 10 2" xfId="48"/>
+    <cellStyle name="Hyperlink 10 3" xfId="49"/>
+    <cellStyle name="Hyperlink 11" xfId="50"/>
+    <cellStyle name="Hyperlink 11 2" xfId="51"/>
+    <cellStyle name="Hyperlink 11 3" xfId="52"/>
+    <cellStyle name="Hyperlink 12" xfId="53"/>
+    <cellStyle name="Hyperlink 12 2" xfId="54"/>
+    <cellStyle name="Hyperlink 12 3" xfId="55"/>
+    <cellStyle name="Hyperlink 13" xfId="56"/>
+    <cellStyle name="Hyperlink 13 2" xfId="57"/>
+    <cellStyle name="Hyperlink 13 3" xfId="58"/>
+    <cellStyle name="Hyperlink 14" xfId="59"/>
+    <cellStyle name="Hyperlink 14 2" xfId="60"/>
+    <cellStyle name="Hyperlink 14 3" xfId="61"/>
+    <cellStyle name="Hyperlink 15" xfId="62"/>
+    <cellStyle name="Hyperlink 15 2" xfId="63"/>
+    <cellStyle name="Hyperlink 15 3" xfId="64"/>
+    <cellStyle name="Hyperlink 16" xfId="65"/>
+    <cellStyle name="Hyperlink 16 2" xfId="66"/>
+    <cellStyle name="Hyperlink 16 3" xfId="67"/>
+    <cellStyle name="Hyperlink 17" xfId="68"/>
+    <cellStyle name="Hyperlink 17 2" xfId="69"/>
+    <cellStyle name="Hyperlink 17 3" xfId="70"/>
+    <cellStyle name="Hyperlink 18" xfId="71"/>
+    <cellStyle name="Hyperlink 18 2" xfId="72"/>
+    <cellStyle name="Hyperlink 18 3" xfId="73"/>
+    <cellStyle name="Hyperlink 19" xfId="74"/>
+    <cellStyle name="Hyperlink 19 2" xfId="75"/>
+    <cellStyle name="Hyperlink 19 3" xfId="76"/>
+    <cellStyle name="Hyperlink 2" xfId="11"/>
+    <cellStyle name="Hyperlink 2 2" xfId="78"/>
+    <cellStyle name="Hyperlink 2 3" xfId="79"/>
+    <cellStyle name="Hyperlink 2 4" xfId="77"/>
+    <cellStyle name="Hyperlink 20" xfId="80"/>
+    <cellStyle name="Hyperlink 20 2" xfId="81"/>
+    <cellStyle name="Hyperlink 20 3" xfId="82"/>
+    <cellStyle name="Hyperlink 21" xfId="83"/>
+    <cellStyle name="Hyperlink 21 2" xfId="84"/>
+    <cellStyle name="Hyperlink 21 3" xfId="85"/>
+    <cellStyle name="Hyperlink 22" xfId="86"/>
+    <cellStyle name="Hyperlink 22 2" xfId="87"/>
+    <cellStyle name="Hyperlink 22 3" xfId="88"/>
+    <cellStyle name="Hyperlink 23" xfId="89"/>
+    <cellStyle name="Hyperlink 23 2" xfId="90"/>
+    <cellStyle name="Hyperlink 23 3" xfId="91"/>
+    <cellStyle name="Hyperlink 24" xfId="92"/>
+    <cellStyle name="Hyperlink 25" xfId="93"/>
+    <cellStyle name="Hyperlink 26" xfId="94"/>
+    <cellStyle name="Hyperlink 27" xfId="95"/>
+    <cellStyle name="Hyperlink 28" xfId="96"/>
+    <cellStyle name="Hyperlink 29" xfId="97"/>
+    <cellStyle name="Hyperlink 3" xfId="98"/>
+    <cellStyle name="Hyperlink 3 2" xfId="99"/>
+    <cellStyle name="Hyperlink 3 3" xfId="100"/>
+    <cellStyle name="Hyperlink 30" xfId="101"/>
+    <cellStyle name="Hyperlink 31" xfId="102"/>
+    <cellStyle name="Hyperlink 32" xfId="103"/>
+    <cellStyle name="Hyperlink 33" xfId="104"/>
+    <cellStyle name="Hyperlink 33 2" xfId="105"/>
+    <cellStyle name="Hyperlink 33 3" xfId="106"/>
+    <cellStyle name="Hyperlink 34" xfId="107"/>
+    <cellStyle name="Hyperlink 34 2" xfId="108"/>
+    <cellStyle name="Hyperlink 34 3" xfId="109"/>
+    <cellStyle name="Hyperlink 34 4" xfId="110"/>
+    <cellStyle name="Hyperlink 34 5" xfId="111"/>
+    <cellStyle name="Hyperlink 4" xfId="112"/>
+    <cellStyle name="Hyperlink 4 2" xfId="113"/>
+    <cellStyle name="Hyperlink 4 3" xfId="114"/>
+    <cellStyle name="Hyperlink 5" xfId="115"/>
+    <cellStyle name="Hyperlink 5 2" xfId="116"/>
+    <cellStyle name="Hyperlink 5 3" xfId="117"/>
+    <cellStyle name="Hyperlink 6" xfId="118"/>
+    <cellStyle name="Hyperlink 6 2" xfId="119"/>
+    <cellStyle name="Hyperlink 6 3" xfId="120"/>
+    <cellStyle name="Hyperlink 7" xfId="121"/>
+    <cellStyle name="Hyperlink 7 2" xfId="122"/>
+    <cellStyle name="Hyperlink 7 3" xfId="123"/>
+    <cellStyle name="Hyperlink 8" xfId="124"/>
+    <cellStyle name="Hyperlink 8 2" xfId="125"/>
+    <cellStyle name="Hyperlink 8 3" xfId="126"/>
+    <cellStyle name="Hyperlink 9" xfId="127"/>
+    <cellStyle name="Hyperlink 9 2" xfId="128"/>
+    <cellStyle name="Hyperlink 9 3" xfId="129"/>
+    <cellStyle name="Input 2" xfId="130"/>
+    <cellStyle name="Linked" xfId="131"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="15" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="Normal 2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="132" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="159" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="Normal 2 2 2 2 2" xfId="181" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="Normal 2 2 2 2 2 2" xfId="225" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="Normal 2 2 2 2 3" xfId="203" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="Normal 2 2 2 3" xfId="170" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="Normal 2 2 2 3 2" xfId="214" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="Normal 2 2 2 4" xfId="192" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="Normal 3" xfId="133" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="Normal 4" xfId="134" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="Normal 5" xfId="135" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="Normal 6" xfId="136" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="Normal 6 2" xfId="160" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="Normal 6 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="226" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="Normal 6 2 3" xfId="204" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="Normal 6 3" xfId="171" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="Normal 6 3 2" xfId="215" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="Normal 6 4" xfId="193" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="Normal 7" xfId="137" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="Normal 8" xfId="138" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="Normal Small" xfId="139" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="Percent 2" xfId="140" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="Percent 2 2" xfId="141" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="Percent 2 3" xfId="142" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="Percent 2 4" xfId="161" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="Percent 2 4 2" xfId="183" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="Percent 2 4 2 2" xfId="227" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="Percent 2 4 3" xfId="205" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="Percent 2 5" xfId="172" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="Percent 2 5 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="Percent 2 6" xfId="194" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="Percent 3" xfId="143" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="Percent 3 2" xfId="144" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="Results" xfId="145" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="Section Break" xfId="12" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="Section Break: parent row" xfId="13" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="Table title" xfId="1" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="Title 2" xfId="146" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="Title 3" xfId="147" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="Unit" xfId="148" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="UserInput" xfId="149" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="Variable" xfId="150" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Normal 2" xfId="15"/>
+    <cellStyle name="Normal 2 2" xfId="14"/>
+    <cellStyle name="Normal 2 2 2" xfId="132"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="159"/>
+    <cellStyle name="Normal 2 2 2 2 2" xfId="181"/>
+    <cellStyle name="Normal 2 2 2 2 2 2" xfId="225"/>
+    <cellStyle name="Normal 2 2 2 2 3" xfId="203"/>
+    <cellStyle name="Normal 2 2 2 3" xfId="170"/>
+    <cellStyle name="Normal 2 2 2 3 2" xfId="214"/>
+    <cellStyle name="Normal 2 2 2 4" xfId="192"/>
+    <cellStyle name="Normal 3" xfId="133"/>
+    <cellStyle name="Normal 4" xfId="134"/>
+    <cellStyle name="Normal 5" xfId="135"/>
+    <cellStyle name="Normal 6" xfId="136"/>
+    <cellStyle name="Normal 6 2" xfId="160"/>
+    <cellStyle name="Normal 6 2 2" xfId="182"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="226"/>
+    <cellStyle name="Normal 6 2 3" xfId="204"/>
+    <cellStyle name="Normal 6 3" xfId="171"/>
+    <cellStyle name="Normal 6 3 2" xfId="215"/>
+    <cellStyle name="Normal 6 4" xfId="193"/>
+    <cellStyle name="Normal 7" xfId="137"/>
+    <cellStyle name="Normal 8" xfId="138"/>
+    <cellStyle name="Normal Small" xfId="139"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Percent 2" xfId="140"/>
+    <cellStyle name="Percent 2 2" xfId="141"/>
+    <cellStyle name="Percent 2 3" xfId="142"/>
+    <cellStyle name="Percent 2 4" xfId="161"/>
+    <cellStyle name="Percent 2 4 2" xfId="183"/>
+    <cellStyle name="Percent 2 4 2 2" xfId="227"/>
+    <cellStyle name="Percent 2 4 3" xfId="205"/>
+    <cellStyle name="Percent 2 5" xfId="172"/>
+    <cellStyle name="Percent 2 5 2" xfId="216"/>
+    <cellStyle name="Percent 2 6" xfId="194"/>
+    <cellStyle name="Percent 3" xfId="143"/>
+    <cellStyle name="Percent 3 2" xfId="144"/>
+    <cellStyle name="Results" xfId="145"/>
+    <cellStyle name="Section Break" xfId="12"/>
+    <cellStyle name="Section Break: parent row" xfId="13"/>
+    <cellStyle name="Table title" xfId="1"/>
+    <cellStyle name="Title 2" xfId="146"/>
+    <cellStyle name="Title 3" xfId="147"/>
+    <cellStyle name="Unit" xfId="148"/>
+    <cellStyle name="UserInput" xfId="149"/>
+    <cellStyle name="Variable" xfId="150"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1435,11 +1441,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Table Style 1" pivot="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="3"/>
       <tableStyleElement type="headerRow" dxfId="2"/>
     </tableStyle>
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1668,7 +1674,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1743,23 +1749,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1795,23 +1784,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1987,23 +1959,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="78.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="78.53125" style="2" customWidth="1"/>
     <col min="3" max="3" width="54.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="77.53125" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="56.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.1328125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="10.6640625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="2"/>
+    <col min="12" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2049,7 +2021,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" ht="28.8">
+    <row r="7" spans="1:11" ht="28.5">
       <c r="B7" s="22" t="s">
         <v>107</v>
       </c>
@@ -2075,7 +2047,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" ht="28.8">
+    <row r="9" spans="1:11" ht="28.5">
       <c r="B9" s="22" t="s">
         <v>108</v>
       </c>
@@ -2231,7 +2203,7 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" ht="28.8">
+    <row r="21" spans="1:11" ht="28.5">
       <c r="A21" s="5"/>
       <c r="B21" s="22" t="s">
         <v>107</v>
@@ -2259,7 +2231,7 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" ht="28.8">
+    <row r="23" spans="1:11" ht="28.5">
       <c r="A23" s="5"/>
       <c r="B23" s="22" t="s">
         <v>108</v>
@@ -2365,7 +2337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="28.8">
+    <row r="36" spans="1:2" ht="28.5">
       <c r="A36" s="5"/>
       <c r="B36" s="22" t="s">
         <v>107</v>
@@ -2377,7 +2349,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="28.8">
+    <row r="38" spans="1:2" ht="28.5">
       <c r="A38" s="5"/>
       <c r="B38" s="22" t="s">
         <v>108</v>
@@ -2763,22 +2735,22 @@
       </c>
     </row>
     <row r="75" spans="1:11" ht="15" customHeight="1">
-      <c r="A75" s="36"/>
+      <c r="A75" s="37"/>
       <c r="B75" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-    </row>
-    <row r="76" spans="1:11" ht="13.2" customHeight="1">
-      <c r="A76" s="36"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+    </row>
+    <row r="76" spans="1:11" ht="13.25" customHeight="1">
+      <c r="A76" s="37"/>
       <c r="B76" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-    </row>
-    <row r="77" spans="1:11" ht="13.2" customHeight="1">
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+    </row>
+    <row r="77" spans="1:11" ht="13.25" customHeight="1">
       <c r="A77" s="31"/>
       <c r="C77" s="31"/>
       <c r="D77" s="31"/>
@@ -2831,9 +2803,9 @@
     <mergeCell ref="A75:A76"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B31" r:id="rId2" xr:uid="{D43D7AD6-251B-49A3-BA96-2770C631E7F6}"/>
-    <hyperlink ref="B45" r:id="rId3" xr:uid="{67B8F900-28B8-43B1-B57C-E32ABBF05B8E}"/>
+    <hyperlink ref="B16" r:id="rId1"/>
+    <hyperlink ref="B31" r:id="rId2"/>
+    <hyperlink ref="B45" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -2841,22 +2813,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B6ADDD-9842-4644-B731-66EF617373E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" style="18" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="18" customWidth="1"/>
     <col min="3" max="3" width="15" style="18" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="18" customWidth="1"/>
-    <col min="5" max="7" width="8.88671875" style="18"/>
-    <col min="8" max="8" width="10.88671875" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="18"/>
+    <col min="4" max="4" width="13.19921875" style="18" customWidth="1"/>
+    <col min="5" max="7" width="8.86328125" style="18"/>
+    <col min="8" max="8" width="10.86328125" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="8.86328125" style="18"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
@@ -2873,18 +2845,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="27" customHeight="1">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36" t="s">
+      <c r="E5" s="37"/>
+      <c r="F5" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="19" t="s">
         <v>58</v>
       </c>
@@ -3673,24 +3645,24 @@
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="37" t="str">
+      <c r="B54" s="38" t="str">
         <f>'CCaMC-AFOaMCpUC'!A1</f>
         <v>Fixed O&amp;M ($/MW)</v>
       </c>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="G54" s="37" t="str">
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="G54" s="38" t="str">
         <f>'CCaMC-VOaMCpUC'!A1</f>
         <v>Variable O&amp;M ($/MWh)</v>
       </c>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-    </row>
-    <row r="55" spans="1:9" ht="28.8">
-      <c r="A55" s="37"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+    </row>
+    <row r="55" spans="1:9" ht="28.5">
+      <c r="A55" s="38"/>
       <c r="B55" s="21" t="s">
         <v>32</v>
       </c>
@@ -3858,19 +3830,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6543B86A-AB5E-437C-BF5B-1A9D4BB7AADD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B38" sqref="B38:C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="25.33203125" style="18" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="18"/>
+    <col min="3" max="3" width="13.46484375" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="8.86328125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4393,36 +4365,36 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A948814-7E97-49CB-B916-F1F28C72D050}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="18"/>
+    <col min="1" max="1" width="8.86328125" style="18"/>
     <col min="2" max="2" width="17.33203125" style="18" customWidth="1"/>
     <col min="3" max="3" width="31" style="18" customWidth="1"/>
     <col min="4" max="5" width="17.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" style="30" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" style="30" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" style="30" customWidth="1"/>
+    <col min="8" max="8" width="22.53125" style="30" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" style="30" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="20.88671875" style="30" customWidth="1"/>
-    <col min="12" max="12" width="28.109375" style="30" customWidth="1"/>
-    <col min="13" max="13" width="19.109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.46484375" style="30" customWidth="1"/>
+    <col min="11" max="11" width="20.86328125" style="30" customWidth="1"/>
+    <col min="12" max="12" width="28.1328125" style="30" customWidth="1"/>
+    <col min="13" max="13" width="19.1328125" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1328125" style="30" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.33203125" style="30" customWidth="1"/>
-    <col min="16" max="16" width="18.88671875" style="30" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" style="30" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" style="30"/>
-    <col min="19" max="16384" width="8.88671875" style="18"/>
+    <col min="16" max="16" width="18.86328125" style="30" customWidth="1"/>
+    <col min="17" max="17" width="16.53125" style="30" customWidth="1"/>
+    <col min="18" max="18" width="8.86328125" style="30"/>
+    <col min="19" max="16384" width="8.86328125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8">
+    <row r="1" spans="1:17" ht="28.5">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -6269,7 +6241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -6279,12 +6251,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.1328125" customWidth="1"/>
+    <col min="3" max="3" width="28.53125" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6564,7 +6536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -6574,11 +6546,11 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="16" customWidth="1"/>
     <col min="2" max="4" width="24" style="16" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="16"/>
+    <col min="5" max="16384" width="9.1328125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6850,36 +6822,36 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K33" sqref="K33:K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
+    <col min="8" max="8" width="22.53125" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="20.88671875" customWidth="1"/>
-    <col min="12" max="12" width="28.109375" customWidth="1"/>
-    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.46484375" customWidth="1"/>
+    <col min="11" max="11" width="20.86328125" customWidth="1"/>
+    <col min="12" max="12" width="28.1328125" customWidth="1"/>
+    <col min="13" max="13" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.33203125" customWidth="1"/>
-    <col min="16" max="16" width="18.88671875" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" customWidth="1"/>
+    <col min="16" max="16" width="18.86328125" customWidth="1"/>
+    <col min="17" max="17" width="16.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8">
+    <row r="1" spans="1:17" ht="28.5">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -6952,11 +6924,11 @@
         <f>AVERAGE('Capital cost data base'!B22:B23)</f>
         <v>2302000</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="36">
         <f>'Capital cost data base'!B42</f>
         <v>1810000</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="36">
         <f>AVERAGE('Capital cost data base'!B40:B41)</f>
         <v>4800000</v>
       </c>
@@ -6984,7 +6956,7 @@
         <f>I2</f>
         <v>3600000</v>
       </c>
-      <c r="N2" s="27">
+      <c r="N2" s="36">
         <f>'Capital cost data base'!B43</f>
         <v>5000000</v>
       </c>
@@ -7022,12 +6994,10 @@
         <v>2302000</v>
       </c>
       <c r="F3" s="27">
-        <f>(((A3-$A$2)/($A$34-$A$2))*($F$34-$F$2))+$F$2</f>
-        <v>1801781.25</v>
+        <v>0</v>
       </c>
       <c r="G3" s="27">
-        <f>(((A3-$A$2)/($A$34-$A$2))*($G$34-$G$2))+$G$2</f>
-        <v>4701562.5</v>
+        <v>0</v>
       </c>
       <c r="H3" s="27">
         <f>'Capital cost EUA model'!H3</f>
@@ -7054,8 +7024,7 @@
         <v>3565625</v>
       </c>
       <c r="N3" s="4">
-        <f>(((A3-$A$2)/($A$34-$A$2))*($N$34-$N$2))+$N$2</f>
-        <v>4937500</v>
+        <v>0</v>
       </c>
       <c r="O3" s="4">
         <f>'Capital cost EUA model'!O3</f>
@@ -7090,20 +7059,18 @@
         <f t="shared" ref="E4:E33" si="3">(((A4-$A$2)/($A$34-$A$2))*($E$34-$E$2))+$E$2</f>
         <v>2302000</v>
       </c>
-      <c r="F4" s="4">
-        <f t="shared" ref="F4:F33" si="4">(((A4-$A$2)/($A$34-$A$2))*($F$34-$F$2))+$F$2</f>
-        <v>1793562.5</v>
-      </c>
-      <c r="G4" s="4">
-        <f t="shared" ref="G4:G33" si="5">(((A4-$A$2)/($A$34-$A$2))*($G$34-$G$2))+$G$2</f>
-        <v>4603125</v>
+      <c r="F4" s="27">
+        <v>0</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0</v>
       </c>
       <c r="H4" s="4">
         <f>'Capital cost EUA model'!H4</f>
         <v>3385650.5382844037</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I33" si="6">(((A4-$A$2)/($A$34-$A$2))*($I$34-$I$2))+$I$2</f>
+        <f t="shared" ref="I4:I33" si="4">(((A4-$A$2)/($A$34-$A$2))*($I$34-$I$2))+$I$2</f>
         <v>3531250</v>
       </c>
       <c r="J4" s="4">
@@ -7115,16 +7082,15 @@
         <v>624214.22900192463</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L33" si="7">(((A4-$A$2)/($A$34-$A$2))*($L$34-$L$2))+$L$2</f>
+        <f t="shared" ref="L4:L33" si="5">(((A4-$A$2)/($A$34-$A$2))*($L$34-$L$2))+$L$2</f>
         <v>1178125</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" ref="M4:M33" si="8">(((A4-$A$2)/($A$34-$A$2))*($M$34-$M$2))+$M$2</f>
+        <f t="shared" ref="M4:M33" si="6">(((A4-$A$2)/($A$34-$A$2))*($M$34-$M$2))+$M$2</f>
         <v>3531250</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" ref="N4:N33" si="9">(((A4-$A$2)/($A$34-$A$2))*($N$34-$N$2))+$N$2</f>
-        <v>4875000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="4">
         <f>'Capital cost EUA model'!O4</f>
@@ -7135,7 +7101,7 @@
         <v>624214.22900192463</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q33" si="10">(((A4-$A$2)/($A$34-$A$2))*($Q$34-$Q$2))+$Q$2</f>
+        <f t="shared" ref="Q4:Q33" si="7">(((A4-$A$2)/($A$34-$A$2))*($Q$34-$Q$2))+$Q$2</f>
         <v>6997500</v>
       </c>
     </row>
@@ -7159,20 +7125,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F5" s="4">
-        <f t="shared" si="4"/>
-        <v>1785343.75</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="5"/>
-        <v>4504687.5</v>
+      <c r="F5" s="27">
+        <v>0</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0</v>
       </c>
       <c r="H5" s="4">
         <f>'Capital cost EUA model'!H5</f>
         <v>3225647.2510458729</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3496875</v>
       </c>
       <c r="J5" s="4">
@@ -7184,16 +7148,15 @@
         <v>616710.15026315721</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1172187.5</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3496875</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="9"/>
-        <v>4812500</v>
+        <v>0</v>
       </c>
       <c r="O5" s="4">
         <f>'Capital cost EUA model'!O5</f>
@@ -7204,7 +7167,7 @@
         <v>616710.15026315721</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6971250</v>
       </c>
     </row>
@@ -7228,20 +7191,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F6" s="4">
-        <f t="shared" si="4"/>
-        <v>1777125</v>
-      </c>
-      <c r="G6" s="4">
-        <f t="shared" si="5"/>
-        <v>4406250</v>
+      <c r="F6" s="27">
+        <v>0</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f>'Capital cost EUA model'!H6</f>
         <v>3036301.351765865</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3462500</v>
       </c>
       <c r="J6" s="4">
@@ -7253,16 +7214,15 @@
         <v>612109.73017863615</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1166250</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3462500</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="9"/>
-        <v>4750000</v>
+        <v>0</v>
       </c>
       <c r="O6" s="4">
         <f>'Capital cost EUA model'!O6</f>
@@ -7273,7 +7233,7 @@
         <v>612109.73017863615</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6945000</v>
       </c>
     </row>
@@ -7297,20 +7257,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F7" s="4">
-        <f t="shared" si="4"/>
-        <v>1768906.25</v>
-      </c>
-      <c r="G7" s="4">
-        <f t="shared" si="5"/>
-        <v>4307812.5</v>
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0</v>
       </c>
       <c r="H7" s="4">
         <f>'Capital cost EUA model'!H7</f>
         <v>2873999.6430443497</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3428125</v>
       </c>
       <c r="J7" s="4">
@@ -7322,16 +7280,15 @@
         <v>600044.48430360877</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1160312.5</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3428125</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="9"/>
-        <v>4687500</v>
+        <v>0</v>
       </c>
       <c r="O7" s="4">
         <f>'Capital cost EUA model'!O7</f>
@@ -7342,7 +7299,7 @@
         <v>600044.48430360877</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6918750</v>
       </c>
     </row>
@@ -7366,20 +7323,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F8" s="4">
-        <f t="shared" si="4"/>
-        <v>1760687.5</v>
-      </c>
-      <c r="G8" s="4">
-        <f t="shared" si="5"/>
-        <v>4209375</v>
+      <c r="F8" s="27">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0</v>
       </c>
       <c r="H8" s="4">
         <f>'Capital cost EUA model'!H8</f>
         <v>2696940.2860163674</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3393750</v>
       </c>
       <c r="J8" s="4">
@@ -7391,16 +7346,15 @@
         <v>594462.88901983364</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1154375</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3393750</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="9"/>
-        <v>4625000</v>
+        <v>0</v>
       </c>
       <c r="O8" s="4">
         <f>'Capital cost EUA model'!O8</f>
@@ -7411,7 +7365,7 @@
         <v>594462.88901983364</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6892500</v>
       </c>
     </row>
@@ -7435,20 +7389,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F9" s="4">
-        <f t="shared" si="4"/>
-        <v>1752468.75</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" si="5"/>
-        <v>4110937.5</v>
+      <c r="F9" s="27">
+        <v>0</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0</v>
       </c>
       <c r="H9" s="4">
         <f>'Capital cost EUA model'!H9</f>
         <v>2519880.9289883869</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3359375</v>
       </c>
       <c r="J9" s="4">
@@ -7460,16 +7412,15 @@
         <v>591147.174835179</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1148437.5</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3359375</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="9"/>
-        <v>4562500</v>
+        <v>0</v>
       </c>
       <c r="O9" s="4">
         <f>'Capital cost EUA model'!O9</f>
@@ -7480,7 +7431,7 @@
         <v>591147.174835179</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6866250</v>
       </c>
     </row>
@@ -7504,20 +7455,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F10" s="4">
-        <f t="shared" si="4"/>
-        <v>1744250</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" si="5"/>
-        <v>4012500</v>
+      <c r="F10" s="27">
+        <v>0</v>
+      </c>
+      <c r="G10" s="27">
+        <v>0</v>
       </c>
       <c r="H10" s="4">
         <f>'Capital cost EUA model'!H10</f>
         <v>2342821.5719604054</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3325000</v>
       </c>
       <c r="J10" s="4">
@@ -7529,16 +7478,15 @@
         <v>587865.47395385115</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1142500</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3325000</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="9"/>
-        <v>4500000</v>
+        <v>0</v>
       </c>
       <c r="O10" s="4">
         <f>'Capital cost EUA model'!O10</f>
@@ -7549,7 +7497,7 @@
         <v>587865.47395385115</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6840000</v>
       </c>
     </row>
@@ -7573,20 +7521,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F11" s="4">
-        <f t="shared" si="4"/>
-        <v>1736031.25</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="5"/>
-        <v>3914062.5</v>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
       </c>
       <c r="H11" s="4">
         <f>'Capital cost EUA model'!H11</f>
         <v>2165762.214932424</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3290625</v>
       </c>
       <c r="J11" s="4">
@@ -7598,16 +7544,15 @@
         <v>584536.34264332184</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1136562.5</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3290625</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="9"/>
-        <v>4437500</v>
+        <v>0</v>
       </c>
       <c r="O11" s="4">
         <f>'Capital cost EUA model'!O11</f>
@@ -7618,7 +7563,7 @@
         <v>584536.34264332184</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6813750</v>
       </c>
     </row>
@@ -7642,20 +7587,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F12" s="4">
-        <f t="shared" si="4"/>
-        <v>1727812.5</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" si="5"/>
-        <v>3815625</v>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
+        <v>0</v>
       </c>
       <c r="H12" s="4">
         <f>'Capital cost EUA model'!H12</f>
         <v>1988702.8579044417</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3256250</v>
       </c>
       <c r="J12" s="4">
@@ -7667,16 +7610,15 @@
         <v>581998.08274038043</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1130625</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3256250</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="9"/>
-        <v>4375000</v>
+        <v>0</v>
       </c>
       <c r="O12" s="4">
         <f>'Capital cost EUA model'!O12</f>
@@ -7687,7 +7629,7 @@
         <v>581998.08274038043</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6787500</v>
       </c>
     </row>
@@ -7711,20 +7653,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F13" s="4">
-        <f t="shared" si="4"/>
-        <v>1719593.75</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" si="5"/>
-        <v>3717187.5</v>
+      <c r="F13" s="27">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0</v>
       </c>
       <c r="H13" s="4">
         <f>'Capital cost EUA model'!H13</f>
         <v>1811643.5008764607</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3221875</v>
       </c>
       <c r="J13" s="4">
@@ -7736,16 +7676,15 @@
         <v>578278.05716929329</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1124687.5</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3221875</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" si="9"/>
-        <v>4312500</v>
+        <v>0</v>
       </c>
       <c r="O13" s="4">
         <f>'Capital cost EUA model'!O13</f>
@@ -7756,7 +7695,7 @@
         <v>578278.05716929329</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6761250</v>
       </c>
     </row>
@@ -7780,20 +7719,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F14" s="4">
-        <f t="shared" si="4"/>
-        <v>1711375</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="5"/>
-        <v>3618750</v>
+      <c r="F14" s="27">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27">
+        <v>0</v>
       </c>
       <c r="H14" s="4">
         <f>'Capital cost EUA model'!H14</f>
         <v>1634584.1438484804</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3187500</v>
       </c>
       <c r="J14" s="4">
@@ -7805,16 +7742,15 @@
         <v>576209.76721946476</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1118750</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3187500</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" si="9"/>
-        <v>4250000</v>
+        <v>0</v>
       </c>
       <c r="O14" s="4">
         <f>'Capital cost EUA model'!O14</f>
@@ -7825,7 +7761,7 @@
         <v>576209.76721946476</v>
       </c>
       <c r="Q14" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6735000</v>
       </c>
     </row>
@@ -7849,20 +7785,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F15" s="4">
-        <f t="shared" si="4"/>
-        <v>1703156.25</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="5"/>
-        <v>3520312.5</v>
+      <c r="F15" s="27">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0</v>
       </c>
       <c r="H15" s="4">
         <f>'Capital cost EUA model'!H15</f>
         <v>1618330.0392752115</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3153125</v>
       </c>
       <c r="J15" s="4">
@@ -7874,16 +7808,15 @@
         <v>574331.56907527894</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1112812.5</v>
       </c>
       <c r="M15" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3153125</v>
       </c>
       <c r="N15" s="4">
-        <f t="shared" si="9"/>
-        <v>4187500</v>
+        <v>0</v>
       </c>
       <c r="O15" s="4">
         <f>'Capital cost EUA model'!O15</f>
@@ -7894,7 +7827,7 @@
         <v>574331.56907527894</v>
       </c>
       <c r="Q15" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6708750</v>
       </c>
     </row>
@@ -7918,20 +7851,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F16" s="4">
-        <f t="shared" si="4"/>
-        <v>1694937.5</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="5"/>
-        <v>3421875</v>
+      <c r="F16" s="27">
+        <v>0</v>
+      </c>
+      <c r="G16" s="27">
+        <v>0</v>
       </c>
       <c r="H16" s="4">
         <f>'Capital cost EUA model'!H16</f>
         <v>1602075.9347019426</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3118750</v>
       </c>
       <c r="J16" s="4">
@@ -7943,16 +7874,15 @@
         <v>571701.18391958985</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1106875</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3118750</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="9"/>
-        <v>4125000</v>
+        <v>0</v>
       </c>
       <c r="O16" s="4">
         <f>'Capital cost EUA model'!O16</f>
@@ -7963,7 +7893,7 @@
         <v>571701.18391958985</v>
       </c>
       <c r="Q16" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6682500</v>
       </c>
     </row>
@@ -7987,20 +7917,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F17" s="4">
-        <f t="shared" si="4"/>
-        <v>1686718.75</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="5"/>
-        <v>3323437.5</v>
+      <c r="F17" s="27">
+        <v>0</v>
+      </c>
+      <c r="G17" s="27">
+        <v>0</v>
       </c>
       <c r="H17" s="4">
         <f>'Capital cost EUA model'!H17</f>
         <v>1585821.8301286742</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3084375</v>
       </c>
       <c r="J17" s="4">
@@ -8012,16 +7940,15 @@
         <v>569693.58845712245</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1100937.5</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3084375</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" si="9"/>
-        <v>4062500</v>
+        <v>0</v>
       </c>
       <c r="O17" s="4">
         <f>'Capital cost EUA model'!O17</f>
@@ -8032,7 +7959,7 @@
         <v>569693.58845712245</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6656250</v>
       </c>
     </row>
@@ -8056,20 +7983,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F18" s="4">
-        <f t="shared" si="4"/>
-        <v>1678500</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="5"/>
-        <v>3225000</v>
+      <c r="F18" s="27">
+        <v>0</v>
+      </c>
+      <c r="G18" s="27">
+        <v>0</v>
       </c>
       <c r="H18" s="4">
         <f>'Capital cost EUA model'!H18</f>
         <v>1569567.7255554048</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3050000</v>
       </c>
       <c r="J18" s="4">
@@ -8081,16 +8006,15 @@
         <v>567853.20501669892</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1095000</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3050000</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="9"/>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="O18" s="4">
         <f>'Capital cost EUA model'!O18</f>
@@ -8101,7 +8025,7 @@
         <v>567853.20501669892</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6630000</v>
       </c>
     </row>
@@ -8125,20 +8049,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F19" s="4">
-        <f t="shared" si="4"/>
-        <v>1670281.25</v>
-      </c>
-      <c r="G19" s="4">
-        <f t="shared" si="5"/>
-        <v>3126562.5</v>
+      <c r="F19" s="27">
+        <v>0</v>
+      </c>
+      <c r="G19" s="27">
+        <v>0</v>
       </c>
       <c r="H19" s="4">
         <f>'Capital cost EUA model'!H19</f>
         <v>1553313.6209821361</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3015625</v>
       </c>
       <c r="J19" s="4">
@@ -8150,16 +8072,15 @@
         <v>565652.8865517024</v>
       </c>
       <c r="L19" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1089062.5</v>
       </c>
       <c r="M19" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3015625</v>
       </c>
       <c r="N19" s="4">
-        <f t="shared" si="9"/>
-        <v>3937500</v>
+        <v>0</v>
       </c>
       <c r="O19" s="4">
         <f>'Capital cost EUA model'!O19</f>
@@ -8170,7 +8091,7 @@
         <v>565652.8865517024</v>
       </c>
       <c r="Q19" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6603750</v>
       </c>
     </row>
@@ -8194,20 +8115,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F20" s="4">
-        <f t="shared" si="4"/>
-        <v>1662062.5</v>
-      </c>
-      <c r="G20" s="4">
-        <f t="shared" si="5"/>
-        <v>3028125</v>
+      <c r="F20" s="27">
+        <v>0</v>
+      </c>
+      <c r="G20" s="27">
+        <v>0</v>
       </c>
       <c r="H20" s="4">
         <f>'Capital cost EUA model'!H20</f>
         <v>1537059.5164088674</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2981250</v>
       </c>
       <c r="J20" s="4">
@@ -8219,16 +8138,15 @@
         <v>563481.86641461716</v>
       </c>
       <c r="L20" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1083125</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2981250</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" si="9"/>
-        <v>3875000</v>
+        <v>0</v>
       </c>
       <c r="O20" s="4">
         <f>'Capital cost EUA model'!O20</f>
@@ -8239,7 +8157,7 @@
         <v>563481.86641461716</v>
       </c>
       <c r="Q20" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6577500</v>
       </c>
     </row>
@@ -8263,20 +8181,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F21" s="4">
-        <f t="shared" si="4"/>
-        <v>1653843.75</v>
-      </c>
-      <c r="G21" s="4">
-        <f t="shared" si="5"/>
-        <v>2929687.5</v>
+      <c r="F21" s="27">
+        <v>0</v>
+      </c>
+      <c r="G21" s="27">
+        <v>0</v>
       </c>
       <c r="H21" s="4">
         <f>'Capital cost EUA model'!H21</f>
         <v>1520805.4118355988</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2946875</v>
       </c>
       <c r="J21" s="4">
@@ -8288,16 +8204,15 @@
         <v>561620.3608197727</v>
       </c>
       <c r="L21" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1077187.5</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2946875</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="9"/>
-        <v>3812500</v>
+        <v>0</v>
       </c>
       <c r="O21" s="4">
         <f>'Capital cost EUA model'!O21</f>
@@ -8308,7 +8223,7 @@
         <v>561620.3608197727</v>
       </c>
       <c r="Q21" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6551250</v>
       </c>
     </row>
@@ -8332,20 +8247,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F22" s="4">
-        <f t="shared" si="4"/>
-        <v>1645625</v>
-      </c>
-      <c r="G22" s="4">
-        <f t="shared" si="5"/>
-        <v>2831250</v>
+      <c r="F22" s="27">
+        <v>0</v>
+      </c>
+      <c r="G22" s="27">
+        <v>0</v>
       </c>
       <c r="H22" s="4">
         <f>'Capital cost EUA model'!H22</f>
         <v>1504551.3072623296</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2912500</v>
       </c>
       <c r="J22" s="4">
@@ -8357,16 +8270,15 @@
         <v>560491.22277389863</v>
       </c>
       <c r="L22" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1071250</v>
       </c>
       <c r="M22" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2912500</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="9"/>
-        <v>3750000</v>
+        <v>0</v>
       </c>
       <c r="O22" s="4">
         <f>'Capital cost EUA model'!O22</f>
@@ -8377,7 +8289,7 @@
         <v>560491.22277389863</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6525000</v>
       </c>
     </row>
@@ -8401,20 +8313,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F23" s="4">
-        <f t="shared" si="4"/>
-        <v>1637406.25</v>
-      </c>
-      <c r="G23" s="4">
-        <f t="shared" si="5"/>
-        <v>2732812.5</v>
+      <c r="F23" s="27">
+        <v>0</v>
+      </c>
+      <c r="G23" s="27">
+        <v>0</v>
       </c>
       <c r="H23" s="4">
         <f>'Capital cost EUA model'!H23</f>
         <v>1488297.2026890602</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2878125</v>
       </c>
       <c r="J23" s="4">
@@ -8426,16 +8336,15 @@
         <v>559063.31435958087</v>
       </c>
       <c r="L23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1065312.5</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2878125</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="9"/>
-        <v>3687500</v>
+        <v>0</v>
       </c>
       <c r="O23" s="4">
         <f>'Capital cost EUA model'!O23</f>
@@ -8446,7 +8355,7 @@
         <v>559063.31435958087</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6498750</v>
       </c>
     </row>
@@ -8470,20 +8379,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F24" s="4">
-        <f t="shared" si="4"/>
-        <v>1629187.5</v>
-      </c>
-      <c r="G24" s="4">
-        <f t="shared" si="5"/>
-        <v>2634375</v>
+      <c r="F24" s="27">
+        <v>0</v>
+      </c>
+      <c r="G24" s="27">
+        <v>0</v>
       </c>
       <c r="H24" s="4">
         <f>'Capital cost EUA model'!H24</f>
         <v>1472043.098115792</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2843750</v>
       </c>
       <c r="J24" s="4">
@@ -8495,16 +8402,15 @@
         <v>557705.69637035497</v>
       </c>
       <c r="L24" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1059375</v>
       </c>
       <c r="M24" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2843750</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="9"/>
-        <v>3625000</v>
+        <v>0</v>
       </c>
       <c r="O24" s="4">
         <f>'Capital cost EUA model'!O24</f>
@@ -8515,7 +8421,7 @@
         <v>557705.69637035497</v>
       </c>
       <c r="Q24" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6472500</v>
       </c>
     </row>
@@ -8539,20 +8445,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F25" s="4">
-        <f t="shared" si="4"/>
-        <v>1620968.75</v>
-      </c>
-      <c r="G25" s="4">
-        <f t="shared" si="5"/>
-        <v>2535937.5</v>
+      <c r="F25" s="27">
+        <v>0</v>
+      </c>
+      <c r="G25" s="27">
+        <v>0</v>
       </c>
       <c r="H25" s="4">
         <f>'Capital cost EUA model'!H25</f>
         <v>1455788.9935425231</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2809375</v>
       </c>
       <c r="J25" s="4">
@@ -8564,16 +8468,15 @@
         <v>556922.89340897254</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1053437.5</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2809375</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="9"/>
-        <v>3562500</v>
+        <v>0</v>
       </c>
       <c r="O25" s="4">
         <f>'Capital cost EUA model'!O25</f>
@@ -8584,7 +8487,7 @@
         <v>556922.89340897254</v>
       </c>
       <c r="Q25" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6446250</v>
       </c>
     </row>
@@ -8608,20 +8511,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F26" s="4">
-        <f t="shared" si="4"/>
-        <v>1612750</v>
-      </c>
-      <c r="G26" s="4">
-        <f t="shared" si="5"/>
-        <v>2437500</v>
+      <c r="F26" s="27">
+        <v>0</v>
+      </c>
+      <c r="G26" s="27">
+        <v>0</v>
       </c>
       <c r="H26" s="4">
         <f>'Capital cost EUA model'!H26</f>
         <v>1439534.888969254</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2775000</v>
       </c>
       <c r="J26" s="4">
@@ -8633,16 +8534,15 @@
         <v>554884.21025692218</v>
       </c>
       <c r="L26" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1047500</v>
       </c>
       <c r="M26" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2775000</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" si="9"/>
-        <v>3500000</v>
+        <v>0</v>
       </c>
       <c r="O26" s="4">
         <f>'Capital cost EUA model'!O26</f>
@@ -8653,7 +8553,7 @@
         <v>554884.21025692218</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6420000</v>
       </c>
     </row>
@@ -8677,20 +8577,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F27" s="4">
-        <f t="shared" si="4"/>
-        <v>1604531.25</v>
-      </c>
-      <c r="G27" s="4">
-        <f t="shared" si="5"/>
-        <v>2339062.5</v>
+      <c r="F27" s="27">
+        <v>0</v>
+      </c>
+      <c r="G27" s="27">
+        <v>0</v>
       </c>
       <c r="H27" s="4">
         <f>'Capital cost EUA model'!H27</f>
         <v>1423280.7843959855</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2740625</v>
       </c>
       <c r="J27" s="4">
@@ -8702,16 +8600,15 @@
         <v>554391.38046651601</v>
       </c>
       <c r="L27" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1041562.5</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2740625</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="9"/>
-        <v>3437500</v>
+        <v>0</v>
       </c>
       <c r="O27" s="4">
         <f>'Capital cost EUA model'!O27</f>
@@ -8722,7 +8619,7 @@
         <v>554391.38046651601</v>
       </c>
       <c r="Q27" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6393750</v>
       </c>
     </row>
@@ -8746,20 +8643,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F28" s="4">
-        <f t="shared" si="4"/>
-        <v>1596312.5</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" si="5"/>
-        <v>2240625</v>
+      <c r="F28" s="27">
+        <v>0</v>
+      </c>
+      <c r="G28" s="27">
+        <v>0</v>
       </c>
       <c r="H28" s="4">
         <f>'Capital cost EUA model'!H28</f>
         <v>1407026.6798227169</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2706250</v>
       </c>
       <c r="J28" s="4">
@@ -8771,16 +8666,15 @@
         <v>552471.36324781028</v>
       </c>
       <c r="L28" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1035625</v>
       </c>
       <c r="M28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2706250</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="9"/>
-        <v>3375000</v>
+        <v>0</v>
       </c>
       <c r="O28" s="4">
         <f>'Capital cost EUA model'!O28</f>
@@ -8791,7 +8685,7 @@
         <v>552471.36324781028</v>
       </c>
       <c r="Q28" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6367500</v>
       </c>
     </row>
@@ -8815,20 +8709,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F29" s="4">
-        <f t="shared" si="4"/>
-        <v>1588093.75</v>
-      </c>
-      <c r="G29" s="4">
-        <f t="shared" si="5"/>
-        <v>2142187.5</v>
+      <c r="F29" s="27">
+        <v>0</v>
+      </c>
+      <c r="G29" s="27">
+        <v>0</v>
       </c>
       <c r="H29" s="4">
         <f>'Capital cost EUA model'!H29</f>
         <v>1390772.5752494477</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2671875</v>
       </c>
       <c r="J29" s="4">
@@ -8840,16 +8732,15 @@
         <v>551856.68438044505</v>
       </c>
       <c r="L29" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1029687.5</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2671875</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="9"/>
-        <v>3312500</v>
+        <v>0</v>
       </c>
       <c r="O29" s="4">
         <f>'Capital cost EUA model'!O29</f>
@@ -8860,7 +8751,7 @@
         <v>551856.68438044505</v>
       </c>
       <c r="Q29" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6341250</v>
       </c>
     </row>
@@ -8884,20 +8775,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F30" s="4">
-        <f t="shared" si="4"/>
-        <v>1579875</v>
-      </c>
-      <c r="G30" s="4">
-        <f t="shared" si="5"/>
-        <v>2043750</v>
+      <c r="F30" s="27">
+        <v>0</v>
+      </c>
+      <c r="G30" s="27">
+        <v>0</v>
       </c>
       <c r="H30" s="4">
         <f>'Capital cost EUA model'!H30</f>
         <v>1374518.470676179</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2637500</v>
       </c>
       <c r="J30" s="4">
@@ -8909,16 +8798,15 @@
         <v>550152.42239255458</v>
       </c>
       <c r="L30" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1023750</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2637500</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="9"/>
-        <v>3250000</v>
+        <v>0</v>
       </c>
       <c r="O30" s="4">
         <f>'Capital cost EUA model'!O30</f>
@@ -8929,7 +8817,7 @@
         <v>550152.42239255458</v>
       </c>
       <c r="Q30" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6315000</v>
       </c>
     </row>
@@ -8953,20 +8841,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F31" s="4">
-        <f t="shared" si="4"/>
-        <v>1571656.25</v>
-      </c>
-      <c r="G31" s="4">
-        <f t="shared" si="5"/>
-        <v>1945312.5</v>
+      <c r="F31" s="27">
+        <v>0</v>
+      </c>
+      <c r="G31" s="27">
+        <v>0</v>
       </c>
       <c r="H31" s="4">
         <f>'Capital cost EUA model'!H31</f>
         <v>1358264.3661029099</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2603125</v>
       </c>
       <c r="J31" s="4">
@@ -8978,16 +8864,15 @@
         <v>548960.60343798099</v>
       </c>
       <c r="L31" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1017812.5</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2603125</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="9"/>
-        <v>3187500</v>
+        <v>0</v>
       </c>
       <c r="O31" s="4">
         <f>'Capital cost EUA model'!O31</f>
@@ -8998,7 +8883,7 @@
         <v>548960.60343798099</v>
       </c>
       <c r="Q31" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6288750</v>
       </c>
     </row>
@@ -9022,20 +8907,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F32" s="4">
-        <f t="shared" si="4"/>
-        <v>1563437.5</v>
-      </c>
-      <c r="G32" s="4">
-        <f t="shared" si="5"/>
-        <v>1846875</v>
+      <c r="F32" s="27">
+        <v>0</v>
+      </c>
+      <c r="G32" s="27">
+        <v>0</v>
       </c>
       <c r="H32" s="4">
         <f>'Capital cost EUA model'!H32</f>
         <v>1342010.261529641</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2568750</v>
       </c>
       <c r="J32" s="4">
@@ -9047,16 +8930,15 @@
         <v>547759.99001111533</v>
       </c>
       <c r="L32" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1011875</v>
       </c>
       <c r="M32" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2568750</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="9"/>
-        <v>3125000</v>
+        <v>0</v>
       </c>
       <c r="O32" s="4">
         <f>'Capital cost EUA model'!O32</f>
@@ -9067,7 +8949,7 @@
         <v>547759.99001111533</v>
       </c>
       <c r="Q32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6262500</v>
       </c>
     </row>
@@ -9091,20 +8973,18 @@
         <f t="shared" si="3"/>
         <v>2302000</v>
       </c>
-      <c r="F33" s="4">
-        <f t="shared" si="4"/>
-        <v>1555218.75</v>
-      </c>
-      <c r="G33" s="4">
-        <f t="shared" si="5"/>
-        <v>1748437.5</v>
+      <c r="F33" s="27">
+        <v>0</v>
+      </c>
+      <c r="G33" s="27">
+        <v>0</v>
       </c>
       <c r="H33" s="4">
         <f>'Capital cost EUA model'!H33</f>
         <v>1325756.1569563723</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2534375</v>
       </c>
       <c r="J33" s="4">
@@ -9116,16 +8996,15 @@
         <v>546510.49006492062</v>
       </c>
       <c r="L33" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1005937.5</v>
       </c>
       <c r="M33" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2534375</v>
       </c>
       <c r="N33" s="4">
-        <f t="shared" si="9"/>
-        <v>3062500</v>
+        <v>0</v>
       </c>
       <c r="O33" s="4">
         <f>'Capital cost EUA model'!O33</f>
@@ -9136,7 +9015,7 @@
         <v>546510.49006492062</v>
       </c>
       <c r="Q33" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>6236250</v>
       </c>
     </row>
@@ -9161,12 +9040,10 @@
         <v>2302000</v>
       </c>
       <c r="F34" s="27">
-        <f>'Capital cost data base'!C42</f>
-        <v>1547000</v>
-      </c>
-      <c r="G34" s="4">
-        <f>AVERAGE('Capital cost data base'!C40:C41)</f>
-        <v>1650000</v>
+        <v>0</v>
+      </c>
+      <c r="G34" s="27">
+        <v>0</v>
       </c>
       <c r="H34" s="4">
         <f>'Capital cost EUA model'!H34</f>
@@ -9180,18 +9057,20 @@
         <f>'Capital cost EUA model'!J34</f>
         <v>668659.39583219984</v>
       </c>
-      <c r="K34" s="4"/>
+      <c r="K34" s="4">
+        <f>'Capital cost EUA model'!K34</f>
+        <v>541058.41525406053</v>
+      </c>
       <c r="L34" s="4">
         <f>'Capital cost data base'!C16</f>
         <v>1000000</v>
       </c>
       <c r="M34" s="4">
-        <f t="shared" ref="M34" si="11">I34</f>
+        <f t="shared" ref="M34" si="8">I34</f>
         <v>2500000</v>
       </c>
-      <c r="N34" s="27">
-        <f>'Capital cost data base'!C43</f>
-        <v>3000000</v>
+      <c r="N34" s="4">
+        <v>0</v>
       </c>
       <c r="O34" s="4">
         <f>'Capital cost EUA model'!O34</f>
@@ -9205,6 +9084,10 @@
         <f>'Capital cost data base'!C33</f>
         <v>6210000</v>
       </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:17">
       <c r="B36" s="11"/>

</xml_diff>